<commit_message>
Order and Product and stuff
</commit_message>
<xml_diff>
--- a/Admin and Documentation/DataWeek5.xlsx
+++ b/Admin and Documentation/DataWeek5.xlsx
@@ -1258,10 +1258,10 @@
   <dimension ref="A1:M187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Data Document updates in Excel
</commit_message>
<xml_diff>
--- a/Admin and Documentation/DataWeek5.xlsx
+++ b/Admin and Documentation/DataWeek5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1258,10 +1258,10 @@
   <dimension ref="A1:M187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>